<commit_message>
maj cartes et buttons
</commit_message>
<xml_diff>
--- a/cartes.xlsx
+++ b/cartes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
   <si>
     <t>Zanersky</t>
   </si>
@@ -79,43 +79,55 @@
     <t>Attaques de base F1/R2 - 1/3 - 2/3 - 2/4…</t>
   </si>
   <si>
-    <t>J</t>
-  </si>
-  <si>
     <t>2 Fast 4 You</t>
   </si>
   <si>
-    <t>Votre adversaire est trop lent: vous lui donnez 2 coups de suite</t>
-  </si>
-  <si>
     <t>Second chance</t>
   </si>
   <si>
     <t>Bad Timing</t>
   </si>
   <si>
-    <t>Vous vous défaussez de X cartes</t>
-  </si>
-  <si>
     <t>Death Throw</t>
   </si>
   <si>
-    <t>L'adversaire se défausse de X cartes</t>
-  </si>
-  <si>
     <t>Grizzly Mode</t>
   </si>
   <si>
-    <t>Vos dégats sont augmentés de 50%</t>
-  </si>
-  <si>
     <t>Can't Beart It</t>
   </si>
   <si>
-    <t>Vous faites trembler la terre par énérvement : vous et votre adversaire perdez 4 cartes!</t>
-  </si>
-  <si>
-    <t>Trop rapide! Vous assainez 4 coups de poing de suite. Impossible à bloquer ce coup mais, vous ne faites pas beaucoup de dégats</t>
+    <t>SUPER</t>
+  </si>
+  <si>
+    <t>Usain Bolt</t>
+  </si>
+  <si>
+    <t>Your opponent is too slow: you hit 2 times in this turn</t>
+  </si>
+  <si>
+    <t>You're so fast, you hit your opponent 4 times. Impossible to block but your fists are not strong enough</t>
+  </si>
+  <si>
+    <t>You increase your damages by 50%</t>
+  </si>
+  <si>
+    <t>You make an earthquake: You and your opponent lose 4 cards</t>
+  </si>
+  <si>
+    <t>You discard 4 cards from your hand</t>
+  </si>
+  <si>
+    <t>Your opponent discards 4 cards from their hand</t>
+  </si>
+  <si>
+    <t>Your opponent doesn't see you running behind them. Surprise attack!</t>
+  </si>
+  <si>
+    <t>Dead eye</t>
+  </si>
+  <si>
+    <t>You throw one of your eye and make your opponent vomit some of their life</t>
   </si>
 </sst>
 </file>
@@ -287,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="distributed"/>
@@ -310,9 +322,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="distributed"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="distributed"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="distributed"/>
     </xf>
@@ -361,8 +370,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="distributed"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -724,31 +733,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" style="15" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" style="16" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="1" width="11.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" style="14" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" style="15" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -808,199 +817,211 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
-      <c r="H2" s="14" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="H2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="H4" s="14" t="s">
+      <c r="D4" s="18"/>
+      <c r="H4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="24"/>
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="N7" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="N9" s="14" t="s">
+      <c r="N9" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="N10" s="14" t="s">
+      <c r="N10" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="N11" s="14" t="s">
+      <c r="N11" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="N12" s="14" t="s">
+      <c r="N12" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="F13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="21"/>
+      <c r="L13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13" s="21"/>
+      <c r="P13" s="22"/>
+      <c r="R13" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="E14" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="F13" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="22"/>
-      <c r="L13" s="15" t="s">
+      <c r="I14" s="21"/>
+      <c r="L14" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="N14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O13" s="22"/>
-      <c r="P13" s="23"/>
-      <c r="R13" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="21"/>
-      <c r="E14" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="14" t="s">
+      <c r="O14" s="21"/>
+      <c r="P14" s="22"/>
+      <c r="R14" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="22"/>
-      <c r="L14" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="N14" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="O14" s="22"/>
-      <c r="P14" s="23"/>
-      <c r="R14" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C15" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="O15" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="P15" s="23"/>
+      <c r="F15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="O15" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="P15" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>